<commit_message>
fix: edit cart and change the maximum quantity input
- แก้ไขหน้าแก้รายละเอียดของรถเข็น
- ปรับจำนวนสูงสุดของ QuantityInput ไม่ให้ตันที่ 99
- แก้ validate serial number ของอุปกรณ์ย่อย จาก toast เป็นข้อความใต้ช่อง
- ปรับตำแหน่ง column ของตัวอย่างไฟล์
</commit_message>
<xml_diff>
--- a/app/public/templates/example-template.xlsx
+++ b/app/public/templates/example-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryu/Desktop/ไฟล์ข้อมูลอุปกรณ์ลูก/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63512F9-C798-3D4A-8BC7-5C4978C1B325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C10BF0-4A14-F140-BA1B-15D60E970C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -425,10 +425,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -447,10 +447,10 @@
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -458,10 +458,10 @@
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -469,10 +469,10 @@
     </row>
     <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -480,10 +480,10 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -491,10 +491,10 @@
     </row>
     <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>

</xml_diff>